<commit_message>
updated with category and search options
</commit_message>
<xml_diff>
--- a/RestAPIs.xlsx
+++ b/RestAPIs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>view blog</t>
   </si>
@@ -39,12 +39,6 @@
     <t>User Actions</t>
   </si>
   <si>
-    <t>sign in</t>
-  </si>
-  <si>
-    <t>sign out</t>
-  </si>
-  <si>
     <t>log in</t>
   </si>
   <si>
@@ -153,7 +147,54 @@
     <t>/user/logout</t>
   </si>
   <si>
-    <t>??</t>
+    <t>sign up</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>session token</t>
+  </si>
+  <si>
+    <t>view blogs of an User</t>
+  </si>
+  <si>
+    <t>/blog?UserId={User.Id}</t>
+  </si>
+  <si>
+    <t>JSON - Header:
+User Object</t>
+  </si>
+  <si>
+    <t>JSON - Header:
+User.username</t>
+  </si>
+  <si>
+    <t>200, 500</t>
+  </si>
+  <si>
+    <t>JSON - Header:
+User name, pwd</t>
+  </si>
+  <si>
+    <t>JSON - body:
+blog</t>
+  </si>
+  <si>
+    <t>JSON - body:
+comment</t>
+  </si>
+  <si>
+    <t>view blogs wrt Category</t>
+  </si>
+  <si>
+    <t>/blog?Category={blog.Category}</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>/blog?v={text string}</t>
   </si>
 </sst>
 </file>
@@ -211,11 +252,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,15 +589,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H22"/>
+  <dimension ref="A3:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="36.77734375" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
@@ -565,23 +609,23 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -596,138 +640,138 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -757,45 +801,45 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -803,43 +847,43 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -847,111 +891,177 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>